<commit_message>
Implemented more generalisations and groupings
</commit_message>
<xml_diff>
--- a/data/new/even_more_private_dataD.xlsx
+++ b/data/new/even_more_private_dataD.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H201"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,15 +461,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>citizenship</t>
+          <t>marital_status</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>marital_status</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>party</t>
         </is>
@@ -497,15 +492,10 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -533,15 +523,10 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -569,15 +554,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -605,15 +585,10 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -641,15 +616,10 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -677,15 +647,10 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -713,15 +678,10 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -749,15 +709,10 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -785,15 +740,10 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -821,15 +771,10 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -857,15 +802,10 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -893,15 +833,10 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
         <is>
           <t>Invalid vote</t>
         </is>
@@ -929,15 +864,10 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -965,15 +895,10 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
         <is>
           <t>Invalid vote</t>
         </is>
@@ -1001,15 +926,10 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1037,15 +957,10 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1073,15 +988,10 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1109,15 +1019,10 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1145,15 +1050,10 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1181,15 +1081,10 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1217,15 +1112,10 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1253,15 +1143,10 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1289,15 +1174,10 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1325,15 +1205,10 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1361,15 +1236,10 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1397,15 +1267,10 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1433,15 +1298,10 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1469,15 +1329,10 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1505,15 +1360,10 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1541,15 +1391,10 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1577,15 +1422,10 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1613,15 +1453,10 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1649,15 +1484,10 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1685,15 +1515,10 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1721,15 +1546,10 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1757,15 +1577,10 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1793,15 +1608,10 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1829,15 +1639,10 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1865,15 +1670,10 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1901,15 +1701,10 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1937,15 +1732,10 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1973,15 +1763,10 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
         <is>
           <t>Invalid vote</t>
         </is>
@@ -2009,15 +1794,10 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2045,15 +1825,10 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2081,15 +1856,10 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2117,15 +1887,10 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2153,15 +1918,10 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2189,15 +1949,10 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2225,15 +1980,10 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2261,15 +2011,10 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2297,15 +2042,10 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2333,15 +2073,10 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2369,15 +2104,10 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2405,15 +2135,10 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2441,15 +2166,10 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2477,15 +2197,10 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2513,15 +2228,10 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2549,15 +2259,10 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2585,15 +2290,10 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2621,15 +2321,10 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2657,15 +2352,10 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2693,15 +2383,10 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2729,15 +2414,10 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2765,15 +2445,10 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2801,15 +2476,10 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2837,15 +2507,10 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2873,15 +2538,10 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2909,15 +2569,10 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2945,15 +2600,10 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2981,15 +2631,10 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3017,15 +2662,10 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3053,15 +2693,10 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3089,15 +2724,10 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3125,15 +2755,10 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3161,15 +2786,10 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3197,15 +2817,10 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3233,15 +2848,10 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3269,15 +2879,10 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3305,15 +2910,10 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3341,15 +2941,10 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3377,15 +2972,10 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3413,15 +3003,10 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3449,15 +3034,10 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3485,15 +3065,10 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3521,15 +3096,10 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3557,15 +3127,10 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3593,15 +3158,10 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3629,15 +3189,10 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3665,15 +3220,10 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3701,15 +3251,10 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3737,15 +3282,10 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3773,15 +3313,10 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3809,15 +3344,10 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3845,15 +3375,10 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3881,15 +3406,10 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3917,15 +3437,10 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -3953,15 +3468,10 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -3989,15 +3499,10 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4025,15 +3530,10 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4061,15 +3561,10 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4097,15 +3592,10 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4133,15 +3623,10 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4169,15 +3654,10 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4205,15 +3685,10 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4241,15 +3716,10 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4277,15 +3747,10 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4313,15 +3778,10 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4349,15 +3809,10 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4385,15 +3840,10 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4421,15 +3871,10 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4457,15 +3902,10 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4493,15 +3933,10 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4529,15 +3964,10 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4565,15 +3995,10 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4601,15 +4026,10 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4637,15 +4057,10 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4673,15 +4088,10 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4709,15 +4119,10 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4745,15 +4150,10 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4781,15 +4181,10 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4817,15 +4212,10 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4853,15 +4243,10 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4889,15 +4274,10 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4925,15 +4305,10 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -4961,15 +4336,10 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H126" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -4997,15 +4367,10 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5033,15 +4398,10 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H128" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5069,15 +4429,10 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5105,15 +4460,10 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5141,15 +4491,10 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H131" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5177,15 +4522,10 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H132" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5213,15 +4553,10 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5249,15 +4584,10 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H134" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5285,15 +4615,10 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5321,15 +4646,10 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H136" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5357,15 +4677,10 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H137" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5393,15 +4708,10 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H138" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5429,15 +4739,10 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H139" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5465,15 +4770,10 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H140" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5501,15 +4801,10 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H141" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5537,15 +4832,10 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H142" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5573,15 +4863,10 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H143" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5609,15 +4894,10 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H144" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5645,15 +4925,10 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5681,15 +4956,10 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H146" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5717,15 +4987,10 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H147" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5753,15 +5018,10 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H148" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5789,15 +5049,10 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H149" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5825,15 +5080,10 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H150" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5861,15 +5111,10 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H151" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5897,15 +5142,10 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H152" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -5933,15 +5173,10 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H153" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -5969,15 +5204,10 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6005,15 +5235,10 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H155" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6041,15 +5266,10 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H156" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6077,15 +5297,10 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H157" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6113,15 +5328,10 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H158" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6149,15 +5359,10 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H159" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6185,15 +5390,10 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H160" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6221,15 +5421,10 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H161" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6257,15 +5452,10 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H162" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6293,15 +5483,10 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H163" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6329,15 +5514,10 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H164" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6365,15 +5545,10 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H165" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6401,15 +5576,10 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6437,15 +5607,10 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H167" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6473,15 +5638,10 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H168" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6509,15 +5669,10 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H169" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6545,15 +5700,10 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H170" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6581,15 +5731,10 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H171" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6617,15 +5762,10 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H172" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6653,15 +5793,10 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H173" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6689,15 +5824,10 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
-        <is>
-          <t>Widowed</t>
-        </is>
-      </c>
-      <c r="H174" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6725,15 +5855,10 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H175" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6761,15 +5886,10 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H176" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6797,15 +5917,10 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H177" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6833,15 +5948,10 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H178" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -6869,15 +5979,10 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H179" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6905,15 +6010,10 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H180" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6941,15 +6041,10 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H181" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -6977,15 +6072,10 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H182" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7013,15 +6103,10 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H183" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7049,15 +6134,10 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H184" t="inlineStr">
         <is>
           <t>Invalid vote</t>
         </is>
@@ -7085,15 +6165,10 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H185" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7121,15 +6196,10 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H186" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7157,15 +6227,10 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H187" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7193,15 +6258,10 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H188" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7229,15 +6289,10 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H189" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7265,15 +6320,10 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H190" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7301,15 +6351,10 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H191" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7337,15 +6382,10 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H192" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7373,15 +6413,10 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H193" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7409,15 +6444,10 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H194" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7445,15 +6475,10 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H195" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7481,15 +6506,10 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H196" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7517,15 +6537,10 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H197" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7553,15 +6568,10 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
-        <is>
-          <t>Married/separated</t>
-        </is>
-      </c>
-      <c r="H198" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7589,15 +6599,10 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Ever married</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
-        <is>
-          <t>Divorced</t>
-        </is>
-      </c>
-      <c r="H199" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -7625,15 +6630,10 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Foreign</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H200" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -7661,15 +6661,10 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Never married</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
-        <is>
-          <t>Never married</t>
-        </is>
-      </c>
-      <c r="H201" t="inlineStr">
         <is>
           <t>Green</t>
         </is>

</xml_diff>